<commit_message>
chemical table import (untested)
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_oligocomponent.xlsx
+++ b/rotmic/static/uploadexample_oligocomponent.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -60,12 +60,6 @@
     <t>Clear the example data (except Status and Type columns) before inserting your own data.</t>
   </si>
   <si>
-    <t>Import of modified Cell entries</t>
-  </si>
-  <si>
-    <t>If left empty, names will be auto-generated from plasmid and strain names.</t>
-  </si>
-  <si>
     <t>Templates</t>
   </si>
   <si>
@@ -97,6 +91,9 @@
   </si>
   <si>
     <t>Tm in C</t>
+  </si>
+  <si>
+    <t>Import of Oligonucleotides</t>
   </si>
 </sst>
 </file>
@@ -487,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -506,7 +503,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -514,69 +511,73 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>14</v>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>5</v>
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="10">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="10">
-        <v>62</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>20</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:8">
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="10"/>
     </row>
@@ -585,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="10"/>
     </row>
@@ -594,7 +595,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="10"/>
     </row>
@@ -603,7 +604,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" s="10"/>
     </row>
@@ -612,7 +613,7 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="10"/>
     </row>
@@ -621,7 +622,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="10"/>
     </row>
@@ -630,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" s="10"/>
     </row>
@@ -639,7 +640,7 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E14" s="10"/>
     </row>
@@ -648,7 +649,7 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" s="10"/>
     </row>
@@ -657,7 +658,7 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E16" s="10"/>
     </row>
@@ -666,7 +667,7 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E17" s="10"/>
     </row>
@@ -675,7 +676,7 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" s="10"/>
     </row>
@@ -684,7 +685,7 @@
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" s="10"/>
     </row>
@@ -693,7 +694,7 @@
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E20" s="10"/>
     </row>
@@ -702,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E21" s="10"/>
     </row>
@@ -711,7 +712,7 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E22" s="10"/>
     </row>
@@ -720,7 +721,7 @@
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E23" s="10"/>
     </row>
@@ -729,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E24" s="10"/>
     </row>
@@ -738,7 +739,7 @@
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E25" s="10"/>
     </row>
@@ -747,7 +748,7 @@
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E26" s="10"/>
     </row>
@@ -756,7 +757,7 @@
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E27" s="10"/>
     </row>
@@ -765,7 +766,7 @@
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E28" s="10"/>
     </row>
@@ -774,7 +775,7 @@
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E29" s="10"/>
     </row>
@@ -783,7 +784,7 @@
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E30" s="10"/>
     </row>
@@ -792,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E31" s="10"/>
     </row>
@@ -801,7 +802,7 @@
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E32" s="10"/>
     </row>
@@ -810,7 +811,7 @@
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E33" s="10"/>
     </row>
@@ -819,7 +820,7 @@
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E34" s="10"/>
     </row>
@@ -828,7 +829,7 @@
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E35" s="10"/>
     </row>
@@ -837,7 +838,7 @@
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E36" s="10"/>
     </row>
@@ -846,7 +847,7 @@
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E37" s="10"/>
     </row>
@@ -855,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E38" s="10"/>
     </row>
@@ -864,7 +865,7 @@
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E39" s="10"/>
     </row>
@@ -873,7 +874,7 @@
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E40" s="10"/>
     </row>
@@ -882,7 +883,7 @@
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E41" s="10"/>
     </row>
@@ -891,25 +892,16 @@
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E42" s="10"/>
-    </row>
-    <row r="43" spans="3:5">
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" t="s">
-        <v>18</v>
-      </c>
-      <c r="E43" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C42">
       <formula1>statusChoices</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D42">
       <formula1>typeChoices</formula1>
     </dataValidation>
   </dataValidations>
@@ -960,7 +952,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L5" t="s">
         <v>11</v>
@@ -971,7 +963,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L6" t="s">
         <v>11</v>
@@ -979,10 +971,10 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L7" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
support purification and reverse primer fields in Excel import.
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_oligocomponent.xlsx
+++ b/rotmic/static/uploadexample_oligocomponent.xlsx
@@ -11,6 +11,7 @@
     <sheet name="predefined" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="purificationChoices">predefined!$E$5:$E$9</definedName>
     <definedName name="statusChoices">predefined!$A$5:$A$8</definedName>
     <definedName name="typeChoices">predefined!$C$5:$C$7</definedName>
   </definedNames>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -48,18 +49,12 @@
     <t>available</t>
   </si>
   <si>
-    <t>This worksheet contains pre-defined choices for the input sheet -- do not modify!</t>
-  </si>
-  <si>
     <t>See: http://office.microsoft.com/en-001/excel-help/insert-or-delete-a-drop-down-list-HP010072599.aspx</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Clear the example data (except Status and Type columns) before inserting your own data.</t>
-  </si>
-  <si>
     <t>Templates</t>
   </si>
   <si>
@@ -78,29 +73,65 @@
     <t>ATGCCCGGACTGGCC</t>
   </si>
   <si>
-    <t>mtp0001, sbf0001</t>
-  </si>
-  <si>
     <t>sbo0001</t>
   </si>
   <si>
     <t>mCit_FW</t>
   </si>
   <si>
-    <t>hypothetical</t>
-  </si>
-  <si>
-    <t>Tm in C</t>
-  </si>
-  <si>
     <t>Import of Oligonucleotides</t>
+  </si>
+  <si>
+    <t>Reverse Primers</t>
+  </si>
+  <si>
+    <t>sbp0001, sbf0001</t>
+  </si>
+  <si>
+    <t>This worksheet contains pre-defined choices for the input sheet -- do not modify unless you know what you are doing!</t>
+  </si>
+  <si>
+    <t>Purification</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>desalting</t>
+  </si>
+  <si>
+    <t>Reverse-phase cartridge</t>
+  </si>
+  <si>
+    <t>HPLC</t>
+  </si>
+  <si>
+    <t>PAGE</t>
+  </si>
+  <si>
+    <t>sbo0002</t>
+  </si>
+  <si>
+    <t>mCit_RV</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>CCGATAGGCAATTCC</t>
+  </si>
+  <si>
+    <t>Tm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +159,13 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -180,15 +218,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -197,6 +233,121 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2981325</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="15230475" cy="809626"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Clear the example data before inserting your own data (except Status</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>, Type,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> and Purification columns to</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> preserve the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> drop-down boxes).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Fields marked in </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Bold</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> are required. Rows without any value in the first column will be ignored.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Templates: Comma-seperated</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> list of DNA construct IDs (or names, but using IDs is more safe).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Reverse Primers: Comma-seperated list of other Oligo IDs (or names, see above).</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -484,429 +635,579 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="27.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="8"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="36.7109375" customWidth="1"/>
-    <col min="8" max="8" width="45.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="40.5703125" customWidth="1"/>
+    <col min="10" max="10" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="9">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="I8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="10">
-        <v>62</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:8">
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:8">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="9">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="C15" t="s">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:8">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="3:6">
       <c r="C17" t="s">
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="3:6">
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="3:6">
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="3:6">
       <c r="C20" t="s">
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="3:6">
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="3:6">
       <c r="C22" t="s">
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="3:6">
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="3:6">
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="3:6">
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="3:6">
       <c r="C26" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="3:6">
       <c r="C27" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="3:6">
       <c r="C28" t="s">
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="3:6">
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="3:6">
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="3:6">
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="3:6">
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="3:6">
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="3:6">
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="3:6">
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="3:6">
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="3:6">
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="10"/>
-    </row>
-    <row r="38" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="3:6">
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="3:6">
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="3:6">
       <c r="C40" t="s">
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="3:6">
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" spans="3:5">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="3:6">
       <c r="C42" t="s">
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="3:6">
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="3:6">
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="3:6">
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="9"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C42">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E45">
+      <formula1>purificationChoices</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C45">
       <formula1>statusChoices</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D45">
       <formula1>typeChoices</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="2400" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -915,25 +1216,27 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="3.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
     <col min="10" max="10" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -943,8 +1246,11 @@
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="K4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -952,10 +1258,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
       </c>
       <c r="L5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -963,79 +1272,91 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
       </c>
       <c r="L7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
       <c r="L8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:12">
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
       <c r="L9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="L10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="L11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="L12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="L13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="L14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="L15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="L16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="12:12">
       <c r="L17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="12:12">
       <c r="L18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel Import: immediate commit of parsed entries; fully rely on transaction management for error handling; This means that it is now possible to create reference links between entries of a table.
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_oligocomponent.xlsx
+++ b/rotmic/static/uploadexample_oligocomponent.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -638,7 +638,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -753,6 +753,9 @@
       </c>
       <c r="G9" t="s">
         <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
       </c>
       <c r="I9" t="s">
         <v>31</v>

</xml_diff>